<commit_message>
New Czech version NIS 2 Annex
Update number version, correct is 4
</commit_message>
<xml_diff>
--- a/tools/NIS2/Annex-Implementing-Regulation-of-NIS2-on-T-M-Czech_version.xlsx
+++ b/tools/NIS2/Annex-Implementing-Regulation-of-NIS2-on-T-M-Czech_version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70787FF3-06D5-4AA2-944D-C8368B21F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D8639D-51A3-460B-B596-7757ED550DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B1CC0E7-3315-034F-9C03-0EA36D269167}"/>
   </bookViews>
@@ -6023,7 +6023,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>